<commit_message>
Added log4j logic File
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/testdata.xlsx
+++ b/src/test/resources/Excel/testdata.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="OpenAccountTest" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>firstname</t>
   </si>
@@ -37,6 +37,18 @@
   </si>
   <si>
     <t>Customer added successfully</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>Rupee</t>
+  </si>
+  <si>
+    <t>Mukesh Ambani</t>
   </si>
 </sst>
 </file>
@@ -377,8 +389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,12 +433,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Complete the Project with Runmode
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/testdata.xlsx
+++ b/src/test/resources/Excel/testdata.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
     <sheet name="OpenAccountTest" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="test_suite" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>firstname</t>
   </si>
@@ -49,6 +49,48 @@
   </si>
   <si>
     <t>Mukesh Ambani</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virat </t>
+  </si>
+  <si>
+    <t>Kohli</t>
+  </si>
+  <si>
+    <t>Rakesh</t>
+  </si>
+  <si>
+    <t>Roshan</t>
+  </si>
+  <si>
+    <t>Arjun</t>
+  </si>
+  <si>
+    <t>Kapoor</t>
+  </si>
+  <si>
+    <t>TCID</t>
+  </si>
+  <si>
+    <t>BankManagerLoginTest</t>
+  </si>
+  <si>
+    <t>OpenAccountTest</t>
+  </si>
+  <si>
+    <t>AddCustomerTest</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Runmode</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>runmode</t>
   </si>
 </sst>
 </file>
@@ -387,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -398,7 +440,7 @@
     <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -411,8 +453,11 @@
       <c r="D1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -424,6 +469,60 @@
       </c>
       <c r="D2" t="s">
         <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>12345</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4">
+        <v>879012</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5">
+        <v>231843</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -435,7 +534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -467,12 +566,50 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>